<commit_message>
Process statuses updated & one more status column added for VPS table
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/vps.xlsx
+++ b/storage/app/excel/templates/vps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD089DB5-EFA9-4E83-973C-DAB666AFF21D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D90FF-E00F-4EE8-87CC-B6354E8D7921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t>РУ</t>
   </si>
   <si>
-    <t>Общий СТАТУС Пд</t>
-  </si>
-  <si>
     <t>СТАТУС Пд</t>
   </si>
   <si>
@@ -169,6 +166,12 @@
   </si>
   <si>
     <t>Категория продуктов</t>
+  </si>
+  <si>
+    <t>СТАТУС Пд Ан*</t>
+  </si>
+  <si>
+    <t>Общий Статус</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +247,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -273,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,6 +310,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -584,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV1"/>
+  <dimension ref="A1:AW1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,35 +617,35 @@
     <col min="11" max="11" width="6" style="4" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" style="4" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="8" style="4" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" customWidth="1"/>
-    <col min="25" max="26" width="12" customWidth="1"/>
-    <col min="27" max="27" width="11" customWidth="1"/>
-    <col min="28" max="28" width="8.28515625" customWidth="1"/>
-    <col min="29" max="30" width="11.5703125" customWidth="1"/>
-    <col min="34" max="34" width="6.85546875" customWidth="1"/>
-    <col min="37" max="37" width="8" customWidth="1"/>
-    <col min="38" max="38" width="11" customWidth="1"/>
-    <col min="39" max="40" width="9" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" customWidth="1"/>
-    <col min="42" max="42" width="8.28515625" customWidth="1"/>
-    <col min="43" max="43" width="8.140625" customWidth="1"/>
-    <col min="44" max="44" width="7.42578125" customWidth="1"/>
-    <col min="45" max="45" width="7.28515625" customWidth="1"/>
-    <col min="47" max="47" width="11" customWidth="1"/>
-    <col min="48" max="48" width="10.7109375" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="8" style="4" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="22" width="6.5703125" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.140625" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
+    <col min="26" max="27" width="12" customWidth="1"/>
+    <col min="28" max="28" width="11" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" customWidth="1"/>
+    <col min="30" max="31" width="11.5703125" customWidth="1"/>
+    <col min="35" max="35" width="6.85546875" customWidth="1"/>
+    <col min="38" max="38" width="8" customWidth="1"/>
+    <col min="39" max="39" width="11" customWidth="1"/>
+    <col min="40" max="41" width="9" customWidth="1"/>
+    <col min="42" max="42" width="10.42578125" customWidth="1"/>
+    <col min="43" max="43" width="8.28515625" customWidth="1"/>
+    <col min="44" max="44" width="8.140625" customWidth="1"/>
+    <col min="45" max="45" width="7.42578125" customWidth="1"/>
+    <col min="46" max="46" width="7.28515625" customWidth="1"/>
+    <col min="48" max="48" width="11" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,110 +685,113 @@
       <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="R1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AE1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AO1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AP1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AT1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AU1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AV1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AW1" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Status stage periods limit 5 removed
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/vps.xlsx
+++ b/storage/app/excel/templates/vps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D90FF-E00F-4EE8-87CC-B6354E8D7921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893CBA4D-716D-4894-9558-49DBB8DC0BC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -172,13 +172,40 @@
   </si>
   <si>
     <t>Общий Статус</t>
+  </si>
+  <si>
+    <t>ВП</t>
+  </si>
+  <si>
+    <t>ПО</t>
+  </si>
+  <si>
+    <t>АЦ</t>
+  </si>
+  <si>
+    <t>СЦ</t>
+  </si>
+  <si>
+    <t>Кк</t>
+  </si>
+  <si>
+    <t>КД</t>
+  </si>
+  <si>
+    <t>НПР</t>
+  </si>
+  <si>
+    <t>Р</t>
+  </si>
+  <si>
+    <t>Зя</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,8 +236,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +288,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -277,12 +318,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +365,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -596,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:BF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AV14" sqref="AV14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +700,7 @@
     <col min="49" max="49" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,6 +847,33 @@
       </c>
       <c r="AW1" s="6" t="s">
         <v>46</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Processes status periods spoiled
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/vps.xlsx
+++ b/storage/app/excel/templates/vps.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\home\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893CBA4D-716D-4894-9558-49DBB8DC0BC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB8D2E1-1166-4AE9-A90F-B451213AEF80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Общий Статус</t>
   </si>
   <si>
-    <t>ВП</t>
-  </si>
-  <si>
     <t>ПО</t>
   </si>
   <si>
@@ -189,16 +186,46 @@
     <t>Кк</t>
   </si>
   <si>
-    <t>КД</t>
-  </si>
-  <si>
-    <t>НПР</t>
-  </si>
-  <si>
     <t>Р</t>
   </si>
   <si>
     <t>Зя</t>
+  </si>
+  <si>
+    <t>Вб</t>
+  </si>
+  <si>
+    <t>SВб</t>
+  </si>
+  <si>
+    <t>SПО</t>
+  </si>
+  <si>
+    <t>SАЦ</t>
+  </si>
+  <si>
+    <t>SСЦ</t>
+  </si>
+  <si>
+    <t>ПцКк</t>
+  </si>
+  <si>
+    <t>SПцКк</t>
+  </si>
+  <si>
+    <t>ПцКД</t>
+  </si>
+  <si>
+    <t>SКД</t>
+  </si>
+  <si>
+    <t>ПцР</t>
+  </si>
+  <si>
+    <t>SПцР</t>
+  </si>
+  <si>
+    <t>P-</t>
   </si>
 </sst>
 </file>
@@ -651,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF1"/>
+  <dimension ref="A1:BO1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AV14" sqref="AV14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BO2" sqref="BO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +727,7 @@
     <col min="49" max="49" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,31 +876,58 @@
         <v>46</v>
       </c>
       <c r="AX1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="12" t="s">
+      <c r="BA1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="12" t="s">
+      <c r="BC1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="12" t="s">
+      <c r="BE1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BG1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="BH1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="12" t="s">
+      <c r="BI1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BL1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BM1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="12" t="s">
+      <c r="BN1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO1" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="BD1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" s="12" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>